<commit_message>
Births and deaths checked
</commit_message>
<xml_diff>
--- a/data-raw/Deaths/D2006.xlsx
+++ b/data-raw/Deaths/D2006.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_PhD\Dati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cha\Documents\demItaly\data-raw\Deaths\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -3152,6 +3152,446 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni6" headers="0" adjustColumnWidth="0" connectionId="24" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni10" headers="0" adjustColumnWidth="0" connectionId="40" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni81" headers="0" adjustColumnWidth="0" connectionId="58" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni80" headers="0" adjustColumnWidth="0" connectionId="18" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni74" headers="0" adjustColumnWidth="0" connectionId="60" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni78" headers="0" adjustColumnWidth="0" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni96" headers="0" adjustColumnWidth="0" connectionId="35" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni7" headers="0" adjustColumnWidth="0" connectionId="22" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni94" headers="0" adjustColumnWidth="0" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni20_1" headers="0" adjustColumnWidth="0" connectionId="53" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni3_1" headers="0" adjustColumnWidth="0" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni25" headers="0" adjustColumnWidth="0" connectionId="37" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni11" headers="0" adjustColumnWidth="0" connectionId="38" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni7_1" headers="0" adjustColumnWidth="0" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni83" headers="0" adjustColumnWidth="0" connectionId="66" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni6_1" headers="0" adjustColumnWidth="0" connectionId="54" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni78_1" headers="0" adjustColumnWidth="0" connectionId="76" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni7_2" headers="0" adjustColumnWidth="0" connectionId="64" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni3" headers="0" adjustColumnWidth="0" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni12" headers="0" adjustColumnWidth="0" connectionId="78" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni26" headers="0" adjustColumnWidth="0" connectionId="77" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni9_1" headers="0" adjustColumnWidth="0" connectionId="39" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni72_1" headers="0" adjustColumnWidth="0" connectionId="52" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni9_2" headers="0" adjustColumnWidth="0" connectionId="72" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni8_2" headers="0" adjustColumnWidth="0" connectionId="71" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni95" headers="0" adjustColumnWidth="0" connectionId="67" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni9" headers="0" adjustColumnWidth="0" connectionId="30" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni4" headers="0" adjustColumnWidth="0" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni71" headers="0" adjustColumnWidth="0" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni79_1" headers="0" adjustColumnWidth="0" connectionId="50" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni8" headers="0" adjustColumnWidth="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni88" headers="0" adjustColumnWidth="0" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni24" headers="0" adjustColumnWidth="0" connectionId="69" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni49" headers="0" adjustColumnWidth="0" connectionId="65" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni91_1" headers="0" adjustColumnWidth="0" connectionId="51" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni75" headers="0" adjustColumnWidth="0" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni4_1" headers="0" adjustColumnWidth="0" connectionId="46" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni4_2" headers="0" adjustColumnWidth="0" connectionId="55" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni18" headers="0" adjustColumnWidth="0" connectionId="45" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni5" headers="0" adjustColumnWidth="0" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable46.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni5_1" headers="0" adjustColumnWidth="0" connectionId="23" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable47.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni77_1" headers="0" adjustColumnWidth="0" connectionId="42" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable48.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni82" headers="0" adjustColumnWidth="0" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable49.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni69" headers="0" adjustColumnWidth="0" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni2_1" headers="0" adjustColumnWidth="0" connectionId="47" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable50.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni22" headers="0" adjustColumnWidth="0" connectionId="61" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable51.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni76" headers="0" adjustColumnWidth="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable52.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni43" headers="0" adjustColumnWidth="0" connectionId="41" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable53.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni47" headers="0" adjustColumnWidth="0" connectionId="57" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable54.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni42" headers="0" adjustColumnWidth="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable55.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni73" headers="0" adjustColumnWidth="0" connectionId="20" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable56.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni2" headers="0" adjustColumnWidth="0" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable57.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni84" headers="0" adjustColumnWidth="0" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable58.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni89" headers="0" adjustColumnWidth="0" connectionId="43" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable59.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni97" headers="0" adjustColumnWidth="0" connectionId="75" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni46" headers="0" adjustColumnWidth="0" connectionId="17" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
@@ -3159,7 +3599,119 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable60.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni93" headers="0" adjustColumnWidth="0" connectionId="59" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable61.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni92" headers="0" adjustColumnWidth="0" connectionId="19" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable62.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni17" headers="0" adjustColumnWidth="0" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable63.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni11_1" headers="0" adjustColumnWidth="0" connectionId="80" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable64.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni3_2" headers="0" adjustColumnWidth="0" connectionId="48" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable65.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni19" headers="0" adjustColumnWidth="0" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable66.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni10_2" headers="0" adjustColumnWidth="0" connectionId="79" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable67.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni21" headers="0" adjustColumnWidth="0" connectionId="21" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable68.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni51" headers="0" adjustColumnWidth="0" connectionId="73" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable69.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni85" headers="0" adjustColumnWidth="0" connectionId="74" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni5_2" headers="0" adjustColumnWidth="0" connectionId="56" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable70.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni70" headers="0" adjustColumnWidth="0" connectionId="44" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable71.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni77" headers="0" adjustColumnWidth="0" connectionId="36" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable72.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni23" headers="0" adjustColumnWidth="0" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
+    <queryTableFields/>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable73.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni8_1" headers="0" adjustColumnWidth="0" connectionId="62" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
@@ -3167,39 +3719,7 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni77_1" headers="0" adjustColumnWidth="0" connectionId="42" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni96" headers="0" adjustColumnWidth="0" connectionId="35" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni11_1" headers="0" adjustColumnWidth="0" connectionId="80" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni95" headers="0" adjustColumnWidth="0" connectionId="67" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable74.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni44" headers="0" adjustColumnWidth="0" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
@@ -3207,47 +3727,39 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni5_1" headers="0" adjustColumnWidth="0" connectionId="23" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+<file path=xl/queryTables/queryTable75.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni50" headers="0" adjustColumnWidth="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
   </queryTableRefresh>
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni78" headers="0" adjustColumnWidth="0" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+<file path=xl/queryTables/queryTable76.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni10_1" headers="0" adjustColumnWidth="0" connectionId="70" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
   </queryTableRefresh>
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni3_2" headers="0" adjustColumnWidth="0" connectionId="48" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+<file path=xl/queryTables/queryTable77.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni76_1" headers="0" adjustColumnWidth="0" connectionId="68" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
   </queryTableRefresh>
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni24" headers="0" adjustColumnWidth="0" connectionId="69" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+<file path=xl/queryTables/queryTable78.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni90" headers="0" adjustColumnWidth="0" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
   </queryTableRefresh>
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni82" headers="0" adjustColumnWidth="0" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable79.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni48" headers="0" adjustColumnWidth="0" connectionId="25" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
@@ -3255,39 +3767,15 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni17" headers="0" adjustColumnWidth="0" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni45_1" headers="0" adjustColumnWidth="0" connectionId="49" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
   </queryTableRefresh>
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni8_2" headers="0" adjustColumnWidth="0" connectionId="71" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni49" headers="0" adjustColumnWidth="0" connectionId="65" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni5" headers="0" adjustColumnWidth="0" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable80.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni1" headers="0" adjustColumnWidth="0" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
@@ -3295,496 +3783,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni92" headers="0" adjustColumnWidth="0" connectionId="19" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni9_2" headers="0" adjustColumnWidth="0" connectionId="72" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni2_1" headers="0" adjustColumnWidth="0" connectionId="47" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni93" headers="0" adjustColumnWidth="0" connectionId="59" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni94" headers="0" adjustColumnWidth="0" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni7_2" headers="0" adjustColumnWidth="0" connectionId="64" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni23" headers="0" adjustColumnWidth="0" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni18" headers="0" adjustColumnWidth="0" connectionId="45" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni80" headers="0" adjustColumnWidth="0" connectionId="18" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni97" headers="0" adjustColumnWidth="0" connectionId="75" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni9_1" headers="0" adjustColumnWidth="0" connectionId="39" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni77" headers="0" adjustColumnWidth="0" connectionId="36" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni4_2" headers="0" adjustColumnWidth="0" connectionId="55" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni74" headers="0" adjustColumnWidth="0" connectionId="60" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni72_1" headers="0" adjustColumnWidth="0" connectionId="52" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni10_2" headers="0" adjustColumnWidth="0" connectionId="79" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni88" headers="0" adjustColumnWidth="0" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni90" headers="0" adjustColumnWidth="0" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni89" headers="0" adjustColumnWidth="0" connectionId="43" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni78_1" headers="0" adjustColumnWidth="0" connectionId="76" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni25" headers="0" adjustColumnWidth="0" connectionId="37" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni4_1" headers="0" adjustColumnWidth="0" connectionId="46" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable46.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni76_1" headers="0" adjustColumnWidth="0" connectionId="68" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable47.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni84" headers="0" adjustColumnWidth="0" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable48.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni26" headers="0" adjustColumnWidth="0" connectionId="77" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable49.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni81" headers="0" adjustColumnWidth="0" connectionId="58" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni9" headers="0" adjustColumnWidth="0" connectionId="30" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable50.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni76" headers="0" adjustColumnWidth="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable51.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni6_1" headers="0" adjustColumnWidth="0" connectionId="54" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable52.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni70" headers="0" adjustColumnWidth="0" connectionId="44" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable53.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni8" headers="0" adjustColumnWidth="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable54.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni10" headers="0" adjustColumnWidth="0" connectionId="40" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable55.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni2" headers="0" adjustColumnWidth="0" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable56.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni12" headers="0" adjustColumnWidth="0" connectionId="78" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable57.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni85" headers="0" adjustColumnWidth="0" connectionId="74" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable58.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni75" headers="0" adjustColumnWidth="0" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable59.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni83" headers="0" adjustColumnWidth="0" connectionId="66" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni45_1" headers="0" adjustColumnWidth="0" connectionId="49" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable60.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni19" headers="0" adjustColumnWidth="0" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable61.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni79_1" headers="0" adjustColumnWidth="0" connectionId="50" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable62.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni10_1" headers="0" adjustColumnWidth="0" connectionId="70" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable63.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni73" headers="0" adjustColumnWidth="0" connectionId="20" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable64.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni7_1" headers="0" adjustColumnWidth="0" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable65.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni6" headers="0" adjustColumnWidth="0" connectionId="24" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable66.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni91_1" headers="0" adjustColumnWidth="0" connectionId="51" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable67.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni50" headers="0" adjustColumnWidth="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable68.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni42" headers="0" adjustColumnWidth="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable69.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni71" headers="0" adjustColumnWidth="0" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni43" headers="0" adjustColumnWidth="0" connectionId="41" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable70.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni5_2" headers="0" adjustColumnWidth="0" connectionId="56" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable71.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni22" headers="0" adjustColumnWidth="0" connectionId="61" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable72.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni11" headers="0" adjustColumnWidth="0" connectionId="38" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable73.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni51" headers="0" adjustColumnWidth="0" connectionId="73" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable74.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni4" headers="0" adjustColumnWidth="0" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni6_2" headers="0" adjustColumnWidth="0" connectionId="63" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable76.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni47" headers="0" adjustColumnWidth="0" connectionId="57" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable77.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni3_1" headers="0" adjustColumnWidth="0" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable78.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni21" headers="0" adjustColumnWidth="0" connectionId="21" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable79.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni69" headers="0" adjustColumnWidth="0" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni7" headers="0" adjustColumnWidth="0" connectionId="22" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable80.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni20_1" headers="0" adjustColumnWidth="0" connectionId="53" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
-  <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
-    <queryTableFields/>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatiEsterni3" headers="0" adjustColumnWidth="0" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1">
   <queryTableRefresh preserveSortFilterLayout="0" headersInLastRefresh="0">
     <queryTableFields/>
   </queryTableRefresh>
@@ -4056,7 +4056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -13778,8 +13778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15493,225 +15493,225 @@
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="10">
+      <c r="A24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="8">
+        <v>9</v>
+      </c>
+      <c r="C24" s="8">
         <v>5</v>
       </c>
-      <c r="C24" s="10">
-        <v>2</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G24" s="10">
-        <v>4</v>
-      </c>
-      <c r="H24" s="10">
-        <v>3</v>
-      </c>
-      <c r="I24" s="10">
-        <v>2</v>
-      </c>
-      <c r="J24" s="10">
-        <v>8</v>
-      </c>
-      <c r="K24" s="10">
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>2</v>
+      </c>
+      <c r="G24" s="8">
         <v>6</v>
       </c>
-      <c r="L24" s="10">
-        <v>12</v>
-      </c>
-      <c r="M24" s="10">
-        <v>16</v>
-      </c>
-      <c r="N24" s="10">
-        <v>24</v>
-      </c>
-      <c r="O24" s="10">
-        <v>38</v>
-      </c>
-      <c r="P24" s="10">
-        <v>69</v>
-      </c>
-      <c r="Q24" s="10">
-        <v>76</v>
-      </c>
-      <c r="R24" s="10">
-        <v>115</v>
-      </c>
-      <c r="S24" s="10">
-        <v>209</v>
-      </c>
-      <c r="T24" s="10">
-        <v>411</v>
-      </c>
-      <c r="U24" s="10">
-        <v>352</v>
-      </c>
-      <c r="V24" s="10">
-        <v>362</v>
-      </c>
-      <c r="W24" s="10">
-        <v>142</v>
-      </c>
-      <c r="X24" s="10">
-        <v>30</v>
+      <c r="H24" s="8">
+        <v>7</v>
+      </c>
+      <c r="I24" s="8">
+        <v>5</v>
+      </c>
+      <c r="J24" s="8">
+        <v>13</v>
+      </c>
+      <c r="K24" s="8">
+        <v>13</v>
+      </c>
+      <c r="L24" s="8">
+        <v>20</v>
+      </c>
+      <c r="M24" s="8">
+        <v>34</v>
+      </c>
+      <c r="N24" s="8">
+        <v>54</v>
+      </c>
+      <c r="O24" s="8">
+        <v>102</v>
+      </c>
+      <c r="P24" s="8">
+        <v>130</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>181</v>
+      </c>
+      <c r="R24" s="8">
+        <v>282</v>
+      </c>
+      <c r="S24" s="8">
+        <v>470</v>
+      </c>
+      <c r="T24" s="8">
+        <v>863</v>
+      </c>
+      <c r="U24" s="8">
+        <v>705</v>
+      </c>
+      <c r="V24" s="8">
+        <v>819</v>
+      </c>
+      <c r="W24" s="8">
+        <v>399</v>
+      </c>
+      <c r="X24" s="8">
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="10">
+        <v>5</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="10">
+        <v>4</v>
+      </c>
+      <c r="H25" s="10">
+        <v>3</v>
+      </c>
+      <c r="I25" s="10">
+        <v>2</v>
+      </c>
+      <c r="J25" s="10">
+        <v>8</v>
+      </c>
+      <c r="K25" s="10">
+        <v>6</v>
+      </c>
+      <c r="L25" s="10">
+        <v>12</v>
+      </c>
+      <c r="M25" s="10">
+        <v>16</v>
+      </c>
+      <c r="N25" s="10">
+        <v>24</v>
+      </c>
+      <c r="O25" s="10">
+        <v>38</v>
+      </c>
+      <c r="P25" s="10">
+        <v>69</v>
+      </c>
+      <c r="Q25" s="10">
+        <v>76</v>
+      </c>
+      <c r="R25" s="10">
+        <v>115</v>
+      </c>
+      <c r="S25" s="10">
+        <v>209</v>
+      </c>
+      <c r="T25" s="10">
+        <v>411</v>
+      </c>
+      <c r="U25" s="10">
+        <v>352</v>
+      </c>
+      <c r="V25" s="10">
+        <v>362</v>
+      </c>
+      <c r="W25" s="10">
+        <v>142</v>
+      </c>
+      <c r="X25" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B26" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C26" s="10">
         <v>3</v>
       </c>
-      <c r="D25" s="10">
-        <v>1</v>
-      </c>
-      <c r="E25" s="10">
-        <v>1</v>
-      </c>
-      <c r="F25" s="10">
-        <v>2</v>
-      </c>
-      <c r="G25" s="10">
-        <v>2</v>
-      </c>
-      <c r="H25" s="10">
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>2</v>
+      </c>
+      <c r="G26" s="10">
+        <v>2</v>
+      </c>
+      <c r="H26" s="10">
         <v>4</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I26" s="10">
         <v>3</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J26" s="10">
         <v>5</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K26" s="10">
         <v>7</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L26" s="10">
         <v>8</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M26" s="10">
         <v>18</v>
       </c>
-      <c r="N25" s="10">
+      <c r="N26" s="10">
         <v>30</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O26" s="10">
         <v>64</v>
       </c>
-      <c r="P25" s="10">
+      <c r="P26" s="10">
         <v>61</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="Q26" s="10">
         <v>105</v>
       </c>
-      <c r="R25" s="10">
+      <c r="R26" s="10">
         <v>167</v>
       </c>
-      <c r="S25" s="10">
+      <c r="S26" s="10">
         <v>261</v>
       </c>
-      <c r="T25" s="10">
+      <c r="T26" s="10">
         <v>452</v>
       </c>
-      <c r="U25" s="10">
+      <c r="U26" s="10">
         <v>353</v>
       </c>
-      <c r="V25" s="10">
+      <c r="V26" s="10">
         <v>457</v>
       </c>
-      <c r="W25" s="10">
+      <c r="W26" s="10">
         <v>257</v>
       </c>
-      <c r="X25" s="10">
+      <c r="X26" s="10">
         <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="8">
-        <v>9</v>
-      </c>
-      <c r="C26" s="8">
-        <v>5</v>
-      </c>
-      <c r="D26" s="8">
-        <v>1</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
-        <v>2</v>
-      </c>
-      <c r="G26" s="8">
-        <v>6</v>
-      </c>
-      <c r="H26" s="8">
-        <v>7</v>
-      </c>
-      <c r="I26" s="8">
-        <v>5</v>
-      </c>
-      <c r="J26" s="8">
-        <v>13</v>
-      </c>
-      <c r="K26" s="8">
-        <v>13</v>
-      </c>
-      <c r="L26" s="8">
-        <v>20</v>
-      </c>
-      <c r="M26" s="8">
-        <v>34</v>
-      </c>
-      <c r="N26" s="8">
-        <v>54</v>
-      </c>
-      <c r="O26" s="8">
-        <v>102</v>
-      </c>
-      <c r="P26" s="8">
-        <v>130</v>
-      </c>
-      <c r="Q26" s="8">
-        <v>181</v>
-      </c>
-      <c r="R26" s="8">
-        <v>282</v>
-      </c>
-      <c r="S26" s="8">
-        <v>470</v>
-      </c>
-      <c r="T26" s="8">
-        <v>863</v>
-      </c>
-      <c r="U26" s="8">
-        <v>705</v>
-      </c>
-      <c r="V26" s="8">
-        <v>819</v>
-      </c>
-      <c r="W26" s="8">
-        <v>399</v>
-      </c>
-      <c r="X26" s="8">
-        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>